<commit_message>
initial version of demo
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\june\Idaithalamdemo\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A612D84-F360-4926-893C-558A334499B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C801A750-5500-4088-8112-FEEB07B7E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="66">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -278,12 +278,15 @@
   <si>
     <t>policy_limit_amount=[0].policy_limit_amount</t>
   </si>
+  <si>
+    <t>InsuranceQuoteByDBReject</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +323,15 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,8 +344,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -439,12 +455,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -469,6 +565,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,15 +793,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -704,6 +800,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1068,7 +1173,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}" name="Table1" displayName="Table1" ref="A1:M10" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}" name="Table1" displayName="Table1" ref="A1:M10" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M10" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{44E9C209-0829-4608-A562-A853364EDCA9}" name="TestCaseName" dataDxfId="12"/>
@@ -1388,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,7 +1933,7 @@
     <col min="13" max="13" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1974,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +2011,7 @@
       </c>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1943,7 +2048,7 @@
       </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1980,7 +2085,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2116,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -2044,7 +2149,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="390" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="390" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -2081,7 +2186,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -2114,7 +2219,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>52</v>
       </c>
@@ -2151,7 +2256,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>47</v>
       </c>
@@ -2188,6 +2293,38 @@
       <c r="L10" s="6"/>
       <c r="M10" s="12" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with new version
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\june-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C801A750-5500-4088-8112-FEEB07B7E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE00057-9BEE-4836-B1AA-5DB955802F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -109,9 +109,6 @@
     <t>http://34.66.48.215:8080/customers/[customerId]</t>
   </si>
   <si>
-    <t>{"email":"[email]","password":"[password]"}</t>
-  </si>
-  <si>
     <t>email=[email]</t>
   </si>
   <si>
@@ -125,18 +122,6 @@
   </si>
   <si>
     <t>CustomerSelfServiceAuth</t>
-  </si>
-  <si>
-    <t>GetCustomerPolicyInfo</t>
-  </si>
-  <si>
-    <t>http://34.66.48.215:8090/customers/[customerId]/policies</t>
-  </si>
-  <si>
-    <t>http://34.66.48.215:8080/customers/[customerId]/insurance-quote-requests</t>
-  </si>
-  <si>
-    <t>GetInsuranceQuote</t>
   </si>
   <si>
     <t>{
@@ -182,9 +167,95 @@
     <t>id=[quoteId]</t>
   </si>
   <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>AcceptInsuranceQuote</t>
+  </si>
+  <si>
+    <t>quoteId=id</t>
+  </si>
+  <si>
+    <t>quote</t>
+  </si>
+  <si>
+    <t>{
+    "status": "QUOTE_ACCEPTED" 
+}</t>
+  </si>
+  <si>
+    <t>ReceiveInsuranceQuote</t>
+  </si>
+  <si>
+    <t>RejectInsuranceQuote</t>
+  </si>
+  <si>
+    <t>{
+    "status": "QUOTE_REJECTED" 
+}</t>
+  </si>
+  <si>
+    <t>rejectQuoteId=id</t>
+  </si>
+  <si>
+    <t>http://34.66.48.215:8090/insurance-quote-requests/[rejectQuoteId]</t>
+  </si>
+  <si>
+    <t>id=[rejectQuoteId]</t>
+  </si>
+  <si>
+    <t>ReceiveInsuranceQuoteToReject</t>
+  </si>
+  <si>
+    <t>CreateInsuranceQuoteForReject</t>
+  </si>
+  <si>
+    <t>Csvson</t>
+  </si>
+  <si>
+    <t>jsonpath=statusHistory
+status
+REQUEST_SUBMITTED
+QUOTE_RECEIVED
+QUOTE_REJECTED</t>
+  </si>
+  <si>
+    <t>statusHistory/status
+REQUEST_SUBMITTED\|QUOTE_RECEIVED\|QUOTE_ACCEPTED\|</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>StepInfo</t>
+  </si>
+  <si>
+    <t>verify record</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]
+id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
+i~[quoteId],d~500.00,CHF,d~50000.00</t>
+  </si>
+  <si>
+    <t>policy_limit_amount=[0].policy_limit_amount</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDBReject</t>
+  </si>
+  <si>
+    <t>{"email":"[email]","password":"[password]"}</t>
+  </si>
+  <si>
     <t>{
     "status": "QUOTE_RECEIVED",
-    "expirationDate": "2021-07-21T04:59:00.000Z",
+    "expirationDate": "2021-09-21T04:59:00.000Z",
     "insurancePremium": {
         "amount": 500,
         "currency": "CHF"
@@ -194,92 +265,6 @@
         "currency": "CHF"
     }
 }</t>
-  </si>
-  <si>
-    <t>PATCH</t>
-  </si>
-  <si>
-    <t>AcceptInsuranceQuote</t>
-  </si>
-  <si>
-    <t>quoteId=id</t>
-  </si>
-  <si>
-    <t>quote</t>
-  </si>
-  <si>
-    <t>{
-    "status": "QUOTE_ACCEPTED" 
-}</t>
-  </si>
-  <si>
-    <t>ReceiveInsuranceQuote</t>
-  </si>
-  <si>
-    <t>RejectInsuranceQuote</t>
-  </si>
-  <si>
-    <t>{
-    "status": "QUOTE_REJECTED" 
-}</t>
-  </si>
-  <si>
-    <t>rejectQuoteId=id</t>
-  </si>
-  <si>
-    <t>http://34.66.48.215:8090/insurance-quote-requests/[rejectQuoteId]</t>
-  </si>
-  <si>
-    <t>id=[rejectQuoteId]</t>
-  </si>
-  <si>
-    <t>ReceiveInsuranceQuoteToReject</t>
-  </si>
-  <si>
-    <t>GetInsuranceQuoteReject</t>
-  </si>
-  <si>
-    <t>CreateInsuranceQuoteForReject</t>
-  </si>
-  <si>
-    <t>Csvson</t>
-  </si>
-  <si>
-    <t>jsonpath=statusHistory
-status
-REQUEST_SUBMITTED
-QUOTE_RECEIVED
-QUOTE_REJECTED</t>
-  </si>
-  <si>
-    <t>statusHistory/status
-REQUEST_SUBMITTED\|QUOTE_RECEIVED\|QUOTE_ACCEPTED\|</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>StepInfo</t>
-  </si>
-  <si>
-    <t>verify record</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDB</t>
-  </si>
-  <si>
-    <t>VERIFY</t>
-  </si>
-  <si>
-    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]
-id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
-i~[quoteId],d~500.00,CHF,d~50000.00</t>
-  </si>
-  <si>
-    <t>policy_limit_amount=[0].policy_limit_amount</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDBReject</t>
   </si>
 </sst>
 </file>
@@ -793,6 +778,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -800,15 +794,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1150,8 +1135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N10" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="A1:N10" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N8" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="A1:N8" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{2529773C-869E-4BF0-BA40-3C63A1B9C82E}" name="TestCaseName" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{38B39313-4971-4AB8-90FF-17FEEBD272E2}" name="Type" dataDxfId="29"/>
@@ -1173,8 +1158,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}" name="Table1" displayName="Table1" ref="A1:M10" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:M10" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}" name="Table1" displayName="Table1" ref="A1:M7" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:M7" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{44E9C209-0829-4608-A562-A853364EDCA9}" name="TestCaseName" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{464049FF-A241-416D-81E2-D042C77E613D}" name="Type" dataDxfId="11"/>
@@ -1491,31 +1476,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:N10"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.83984375" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="27.83984375" customWidth="1"/>
+    <col min="5" max="5" width="20.26171875" customWidth="1"/>
+    <col min="6" max="6" width="70.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83984375" customWidth="1"/>
+    <col min="8" max="8" width="16.15625" customWidth="1"/>
+    <col min="9" max="9" width="14.83984375" customWidth="1"/>
+    <col min="10" max="10" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.578125" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="88.85546875" customWidth="1"/>
+    <col min="13" max="13" width="39.578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="88.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1544,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>13</v>
@@ -1556,12 +1541,12 @@
         <v>16</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
@@ -1587,17 +1572,17 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="14"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1624,18 +1609,18 @@
         <v>200</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1662,36 +1647,36 @@
         <v>200</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>12</v>
@@ -1699,31 +1684,37 @@
       <c r="I5" s="6">
         <v>200</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="1:14" ht="390" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>12</v>
@@ -1732,20 +1723,20 @@
         <v>200</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="M6" s="6"/>
       <c r="N6" s="14"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
@@ -1753,15 +1744,15 @@
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="G7" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>12</v>
@@ -1770,121 +1761,49 @@
         <v>200</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="M7" s="6"/>
-      <c r="N7" s="14"/>
+      <c r="N7" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="6">
-        <v>200</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6">
-        <v>200</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="N9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>63</v>
+      <c r="N8" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1894,46 +1813,44 @@
     <hyperlink ref="L3" r:id="rId3" display="email=admin@example.com" xr:uid="{6578FDF2-846E-4A5F-AFC5-42766B4B0470}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{18970103-3D15-4C34-A217-1990C9B8F8E3}"/>
     <hyperlink ref="L2" r:id="rId5" display="email=admin@example.com" xr:uid="{FA7D36A9-A6DA-4DA4-881D-45A3E3E86790}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{11FD1300-06AC-4106-B281-1E29DB2D2F01}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{23FBB02D-840A-46D3-BF20-5482236806EC}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="5" max="5" width="70.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83984375" customWidth="1"/>
+    <col min="7" max="7" width="16.15625" customWidth="1"/>
+    <col min="8" max="8" width="14.83984375" customWidth="1"/>
+    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.578125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1876,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>13</v>
@@ -1971,12 +1888,12 @@
         <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
@@ -2001,17 +1918,17 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -2037,18 +1954,18 @@
         <v>200</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2074,35 +1991,35 @@
         <v>200</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
@@ -2110,30 +2027,36 @@
       <c r="H5" s="6">
         <v>200</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="K5" s="8"/>
-      <c r="L5" s="6"/>
+      <c r="L5" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
@@ -2142,16 +2065,20 @@
         <v>200</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="L6" s="6"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="390" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
@@ -2160,13 +2087,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>12</v>
@@ -2175,156 +2102,49 @@
         <v>200</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="6">
-        <v>200</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6">
-        <v>200</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="6">
-        <v>200</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="12" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="24" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2334,17 +2154,14 @@
     <hyperlink ref="K3" r:id="rId3" display="email=admin@example.com" xr:uid="{924C8EEF-8216-4237-990F-0F5500A53827}"/>
     <hyperlink ref="E4" r:id="rId4" xr:uid="{E21BD94E-4C02-4B13-BFB8-24DF671FBC4B}"/>
     <hyperlink ref="K2" r:id="rId5" display="email=admin@example.com" xr:uid="{2AC9B76B-9478-4CCC-B9EE-AECB42C021D8}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{4A637E5D-E0E0-4FF4-9B85-FCBFC4BCDAD5}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{754EBE1A-9E3F-46A3-86F6-C67B59FF684C}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{9FD1DDE3-0C92-4BE4-9241-79DC041815AC}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{72EB1D07-774C-4B76-9AE3-3751A771F305}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{5F09E6C4-56C4-4CC9-BF31-72583E111233}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{BB9ACE82-6D2D-401D-AEDC-761999503176}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{9FD1DDE3-0C92-4BE4-9241-79DC041815AC}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{5F09E6C4-56C4-4CC9-BF31-72583E111233}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{BB9ACE82-6D2D-401D-AEDC-761999503176}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with new release version
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\june-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\september-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE00057-9BEE-4836-B1AA-5DB955802F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AB00D5-151E-4671-9A54-4E15D5B8673E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -236,9 +236,6 @@
     <t>InsuranceQuoteByDB</t>
   </si>
   <si>
-    <t>VERIFY</t>
-  </si>
-  <si>
     <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]
 id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
 i~[quoteId],d~500.00,CHF,d~50000.00</t>
@@ -253,9 +250,63 @@
     <t>{"email":"[email]","password":"[password]"}</t>
   </si>
   <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>Read Quote information</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [rejectQuoteId]</t>
+  </si>
+  <si>
+    <t>{
+    "statusHistory": [],
+    "customerInfo": {
+        "customerId": "[customerId]",
+        "firstname": "[firstname]",
+        "lastname": "[lastname]",
+        "contactAddress": {
+            "streetAddress": "[streetAddress]",
+            "postalCode": "[postalCode]",
+            "city": "[city]"
+        },
+        "billingAddress": {
+            "streetAddress": "[streetAddress]",
+            "postalCode": "[postalCode]",
+            "city": "[city]"
+        }
+    },
+    "insuranceOptions": {
+        "startDate": "2021-09-20",
+        "insuranceType": "Life Insurance",
+        "deductible": {
+            "amount": 500,
+            "currency": "CHF"
+        }
+    }
+}</t>
+  </si>
+  <si>
     <t>{
     "status": "QUOTE_RECEIVED",
-    "expirationDate": "2021-09-21T04:59:00.000Z",
+    "expirationDate": "2022-09-21T04:59:00.000Z",
+    "insurancePremium": {
+        "amount": 500,
+        "currency": "CHF"
+    },
+    "policyLimit": {
+        "amount": 50000,
+        "currency": "CHF"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "QUOTE_RECEIVED",
+    "expirationDate": "2021-11-21T04:59:00.000Z",
     "insurancePremium": {
         "amount": 500,
         "currency": "CHF"
@@ -336,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -459,19 +510,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -550,13 +588,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1478,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1572,7 +1612,7 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>24</v>
@@ -1726,7 +1766,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>34</v>
@@ -1792,18 +1832,20 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="K8" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="L8" s="8"/>
       <c r="M8" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1827,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1847,10 +1889,10 @@
     <col min="10" max="10" width="54.578125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.15625" customWidth="1"/>
+    <col min="13" max="13" width="34.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1918,7 +1960,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>24</v>
@@ -1928,7 +1970,7 @@
       </c>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1965,7 +2007,7 @@
       </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2002,7 +2044,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -2031,7 +2073,7 @@
         <v>27</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="6" t="s">
@@ -2039,7 +2081,7 @@
       </c>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -2068,7 +2110,7 @@
         <v>27</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>45</v>
@@ -2076,7 +2118,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2115,9 +2157,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>51</v>
@@ -2126,26 +2168,25 @@
         <v>9</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22" t="s">
-        <v>55</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="22"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="J8" s="24" t="s">
+        <v>62</v>
+      </c>
       <c r="K8" s="19"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="24" t="s">
+      <c r="L8" s="19" t="s">
         <v>56</v>
       </c>
+      <c r="M8" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated with Perf setup and Execution option with idaithalam
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\september-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AB00D5-151E-4671-9A54-4E15D5B8673E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89F0D0F-2326-4928-BE2A-3C6CB34B1463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="67">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -290,23 +290,15 @@
 }</t>
   </si>
   <si>
+    <t>expiryDate=SUBSTITUTE(TEXT(NOW()+365, "yyyy-mm-dd HH:mm:ss"), " ", "T");startDate=TEXT(TODAY(),"yyyy-mm-dd")</t>
+  </si>
+  <si>
+    <t>EvaluateFunctionVariables</t>
+  </si>
+  <si>
     <t>{
     "status": "QUOTE_RECEIVED",
-    "expirationDate": "2022-09-21T04:59:00.000Z",
-    "insurancePremium": {
-        "amount": 500,
-        "currency": "CHF"
-    },
-    "policyLimit": {
-        "amount": 50000,
-        "currency": "CHF"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "QUOTE_RECEIVED",
-    "expirationDate": "2021-11-21T04:59:00.000Z",
+    "expirationDate": "[expiryDate].000Z",
     "insurancePremium": {
         "amount": 500,
         "currency": "CHF"
@@ -1516,31 +1508,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+    <sheetView topLeftCell="I4" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83984375" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="27.83984375" customWidth="1"/>
-    <col min="5" max="5" width="20.26171875" customWidth="1"/>
-    <col min="6" max="6" width="70.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83984375" customWidth="1"/>
-    <col min="8" max="8" width="16.15625" customWidth="1"/>
-    <col min="9" max="9" width="14.83984375" customWidth="1"/>
-    <col min="10" max="10" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.578125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="88.83984375" customWidth="1"/>
+    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="88.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1583,8 +1576,11 @@
       <c r="N1" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1621,8 +1617,9 @@
         <v>15</v>
       </c>
       <c r="N2" s="14"/>
+      <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1659,8 +1656,11 @@
         <v>20</v>
       </c>
       <c r="N3" s="14"/>
+      <c r="O3" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1697,8 +1697,9 @@
         <v>30</v>
       </c>
       <c r="N4" s="14"/>
+      <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1735,8 +1736,9 @@
         <v>37</v>
       </c>
       <c r="N5" s="14"/>
+      <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -1766,15 +1768,16 @@
         <v>27</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="14"/>
+      <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -1813,8 +1816,9 @@
       <c r="N7" s="15" t="s">
         <v>50</v>
       </c>
+      <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>54</v>
       </c>
@@ -1869,30 +1873,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="H6" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="16.15625" customWidth="1"/>
-    <col min="8" max="8" width="14.83984375" customWidth="1"/>
-    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.578125" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.9453125" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1932,8 +1937,11 @@
       <c r="M1" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1969,8 +1977,9 @@
         <v>15</v>
       </c>
       <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -2006,8 +2015,11 @@
         <v>20</v>
       </c>
       <c r="M3" s="9"/>
+      <c r="N3" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2043,8 +2055,9 @@
         <v>30</v>
       </c>
       <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:13" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -2080,8 +2093,9 @@
         <v>43</v>
       </c>
       <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -2110,15 +2124,16 @@
         <v>27</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>45</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2156,8 +2171,9 @@
       <c r="M7" s="12" t="s">
         <v>49</v>
       </c>
+      <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>57</v>
       </c>

</xml_diff>